<commit_message>
- many small improvements
</commit_message>
<xml_diff>
--- a/data/sheet/msg_8705.xlsx
+++ b/data/sheet/msg_8705.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4273" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4843" uniqueCount="180">
   <si>
     <t/>
   </si>
@@ -503,6 +503,66 @@
   <si>
     <t>2022-03-21 17:10:29</t>
   </si>
+  <si>
+    <t>2022-03-22 07:53:58</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>2022-03-22 08:10:21</t>
+  </si>
+  <si>
+    <t>2022-03-22 08:21:23</t>
+  </si>
+  <si>
+    <t>2022-03-22 08:28:25</t>
+  </si>
+  <si>
+    <t>2022-03-22 09:23:32</t>
+  </si>
+  <si>
+    <t>2022-03-22 09:52:35</t>
+  </si>
+  <si>
+    <t>2022-03-22 09:57:36</t>
+  </si>
+  <si>
+    <t>2022-03-22 10:03:37</t>
+  </si>
+  <si>
+    <t>2022-03-22 10:26:39</t>
+  </si>
+  <si>
+    <t>2022-03-22 10:29:40</t>
+  </si>
+  <si>
+    <t>2022-03-22 10:43:43</t>
+  </si>
+  <si>
+    <t>2022-03-22 11:01:45</t>
+  </si>
+  <si>
+    <t>2022-03-22 11:06:47</t>
+  </si>
+  <si>
+    <t>2022-03-22 11:17:48</t>
+  </si>
+  <si>
+    <t>2022-03-22 11:23:49</t>
+  </si>
+  <si>
+    <t>2022-03-22 11:54:53</t>
+  </si>
+  <si>
+    <t>2022-03-22 11:59:53</t>
+  </si>
+  <si>
+    <t>2022-03-22 12:40:58</t>
+  </si>
+  <si>
+    <t>2022-03-22 12:43:58</t>
+  </si>
 </sst>
 </file>
 
@@ -854,7 +914,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H143"/>
+  <dimension ref="A1:H162"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4583,6 +4643,500 @@
         <v>255.0</v>
       </c>
     </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>160</v>
+      </c>
+      <c r="B144" t="s">
+        <v>0</v>
+      </c>
+      <c r="C144" t="s">
+        <v>10</v>
+      </c>
+      <c r="D144" t="n">
+        <v>1.647932039E9</v>
+      </c>
+      <c r="E144" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F144" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H144" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>162</v>
+      </c>
+      <c r="B145" t="s">
+        <v>0</v>
+      </c>
+      <c r="C145" t="s">
+        <v>10</v>
+      </c>
+      <c r="D145" t="n">
+        <v>1.647933022E9</v>
+      </c>
+      <c r="E145" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F145" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G145" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H145" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>163</v>
+      </c>
+      <c r="B146" t="s">
+        <v>0</v>
+      </c>
+      <c r="C146" t="s">
+        <v>10</v>
+      </c>
+      <c r="D146" t="n">
+        <v>1.647933684E9</v>
+      </c>
+      <c r="E146" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F146" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G146" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H146" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>164</v>
+      </c>
+      <c r="B147" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147" t="s">
+        <v>10</v>
+      </c>
+      <c r="D147" t="n">
+        <v>1.647934105E9</v>
+      </c>
+      <c r="E147" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F147" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G147" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H147" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>165</v>
+      </c>
+      <c r="B148" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" t="s">
+        <v>10</v>
+      </c>
+      <c r="D148" t="n">
+        <v>1.647937412E9</v>
+      </c>
+      <c r="E148" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G148" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H148" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>166</v>
+      </c>
+      <c r="B149" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" t="s">
+        <v>10</v>
+      </c>
+      <c r="D149" t="n">
+        <v>1.647939156E9</v>
+      </c>
+      <c r="E149" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F149" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G149" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H149" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>167</v>
+      </c>
+      <c r="B150" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150" t="s">
+        <v>10</v>
+      </c>
+      <c r="D150" t="n">
+        <v>1.647939457E9</v>
+      </c>
+      <c r="E150" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F150" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G150" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H150" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>168</v>
+      </c>
+      <c r="B151" t="s">
+        <v>0</v>
+      </c>
+      <c r="C151" t="s">
+        <v>10</v>
+      </c>
+      <c r="D151" t="n">
+        <v>1.647939818E9</v>
+      </c>
+      <c r="E151" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F151" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G151" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H151" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>169</v>
+      </c>
+      <c r="B152" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" t="s">
+        <v>10</v>
+      </c>
+      <c r="D152" t="n">
+        <v>1.6479412E9</v>
+      </c>
+      <c r="E152" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F152" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G152" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H152" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>170</v>
+      </c>
+      <c r="B153" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" t="s">
+        <v>10</v>
+      </c>
+      <c r="D153" t="n">
+        <v>1.647941381E9</v>
+      </c>
+      <c r="E153" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F153" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G153" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H153" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>171</v>
+      </c>
+      <c r="B154" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154" t="s">
+        <v>10</v>
+      </c>
+      <c r="D154" t="n">
+        <v>1.647942224E9</v>
+      </c>
+      <c r="E154" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F154" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G154" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H154" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>172</v>
+      </c>
+      <c r="B155" t="s">
+        <v>0</v>
+      </c>
+      <c r="C155" t="s">
+        <v>10</v>
+      </c>
+      <c r="D155" t="n">
+        <v>1.647943307E9</v>
+      </c>
+      <c r="E155" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F155" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G155" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H155" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>173</v>
+      </c>
+      <c r="B156" t="s">
+        <v>0</v>
+      </c>
+      <c r="C156" t="s">
+        <v>10</v>
+      </c>
+      <c r="D156" t="n">
+        <v>1.647943609E9</v>
+      </c>
+      <c r="E156" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F156" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G156" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H156" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>174</v>
+      </c>
+      <c r="B157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157" t="s">
+        <v>10</v>
+      </c>
+      <c r="D157" t="n">
+        <v>1.64794427E9</v>
+      </c>
+      <c r="E157" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F157" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G157" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H157" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>175</v>
+      </c>
+      <c r="B158" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" t="s">
+        <v>10</v>
+      </c>
+      <c r="D158" t="n">
+        <v>1.647944631E9</v>
+      </c>
+      <c r="E158" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F158" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G158" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H158" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>176</v>
+      </c>
+      <c r="B159" t="s">
+        <v>0</v>
+      </c>
+      <c r="C159" t="s">
+        <v>10</v>
+      </c>
+      <c r="D159" t="n">
+        <v>1.647946495E9</v>
+      </c>
+      <c r="E159" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F159" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G159" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H159" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>177</v>
+      </c>
+      <c r="B160" t="s">
+        <v>0</v>
+      </c>
+      <c r="C160" t="s">
+        <v>10</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1.647946795E9</v>
+      </c>
+      <c r="E160" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F160" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G160" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H160" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>178</v>
+      </c>
+      <c r="B161" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" t="s">
+        <v>10</v>
+      </c>
+      <c r="D161" t="n">
+        <v>1.64794926E9</v>
+      </c>
+      <c r="E161" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F161" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G161" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H161" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>179</v>
+      </c>
+      <c r="B162" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162" t="s">
+        <v>10</v>
+      </c>
+      <c r="D162" t="n">
+        <v>1.64794944E9</v>
+      </c>
+      <c r="E162" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F162" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G162" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H162" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4590,7 +5144,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:L162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -10036,6 +10590,728 @@
         <v>0</v>
       </c>
     </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>160</v>
+      </c>
+      <c r="B144" t="s">
+        <v>0</v>
+      </c>
+      <c r="C144" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D144" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E144" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F144" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G144" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H144" t="s">
+        <v>0</v>
+      </c>
+      <c r="I144" t="s">
+        <v>161</v>
+      </c>
+      <c r="J144" t="s">
+        <v>0</v>
+      </c>
+      <c r="K144" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L144" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>162</v>
+      </c>
+      <c r="B145" t="s">
+        <v>0</v>
+      </c>
+      <c r="C145" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D145" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E145" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F145" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G145" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H145" t="s">
+        <v>0</v>
+      </c>
+      <c r="I145" t="s">
+        <v>161</v>
+      </c>
+      <c r="J145" t="s">
+        <v>0</v>
+      </c>
+      <c r="K145" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L145" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>163</v>
+      </c>
+      <c r="B146" t="s">
+        <v>0</v>
+      </c>
+      <c r="C146" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D146" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E146" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F146" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G146" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H146" t="s">
+        <v>0</v>
+      </c>
+      <c r="I146" t="s">
+        <v>161</v>
+      </c>
+      <c r="J146" t="s">
+        <v>0</v>
+      </c>
+      <c r="K146" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L146" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>164</v>
+      </c>
+      <c r="B147" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D147" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E147" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F147" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G147" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H147" t="s">
+        <v>0</v>
+      </c>
+      <c r="I147" t="s">
+        <v>161</v>
+      </c>
+      <c r="J147" t="s">
+        <v>0</v>
+      </c>
+      <c r="K147" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L147" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>165</v>
+      </c>
+      <c r="B148" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D148" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E148" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G148" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H148" t="s">
+        <v>0</v>
+      </c>
+      <c r="I148" t="s">
+        <v>161</v>
+      </c>
+      <c r="J148" t="s">
+        <v>0</v>
+      </c>
+      <c r="K148" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L148" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>166</v>
+      </c>
+      <c r="B149" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D149" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G149" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H149" t="s">
+        <v>0</v>
+      </c>
+      <c r="I149" t="s">
+        <v>161</v>
+      </c>
+      <c r="J149" t="s">
+        <v>0</v>
+      </c>
+      <c r="K149" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L149" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>167</v>
+      </c>
+      <c r="B150" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D150" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G150" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H150" t="s">
+        <v>0</v>
+      </c>
+      <c r="I150" t="s">
+        <v>161</v>
+      </c>
+      <c r="J150" t="s">
+        <v>0</v>
+      </c>
+      <c r="K150" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L150" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>168</v>
+      </c>
+      <c r="B151" t="s">
+        <v>0</v>
+      </c>
+      <c r="C151" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D151" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F151" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G151" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H151" t="s">
+        <v>0</v>
+      </c>
+      <c r="I151" t="s">
+        <v>161</v>
+      </c>
+      <c r="J151" t="s">
+        <v>0</v>
+      </c>
+      <c r="K151" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L151" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>169</v>
+      </c>
+      <c r="B152" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D152" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E152" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F152" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G152" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H152" t="s">
+        <v>0</v>
+      </c>
+      <c r="I152" t="s">
+        <v>161</v>
+      </c>
+      <c r="J152" t="s">
+        <v>0</v>
+      </c>
+      <c r="K152" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L152" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>170</v>
+      </c>
+      <c r="B153" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D153" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E153" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F153" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G153" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H153" t="s">
+        <v>0</v>
+      </c>
+      <c r="I153" t="s">
+        <v>161</v>
+      </c>
+      <c r="J153" t="s">
+        <v>0</v>
+      </c>
+      <c r="K153" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L153" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>171</v>
+      </c>
+      <c r="B154" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D154" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E154" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F154" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G154" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H154" t="s">
+        <v>0</v>
+      </c>
+      <c r="I154" t="s">
+        <v>161</v>
+      </c>
+      <c r="J154" t="s">
+        <v>0</v>
+      </c>
+      <c r="K154" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L154" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>172</v>
+      </c>
+      <c r="B155" t="s">
+        <v>0</v>
+      </c>
+      <c r="C155" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D155" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E155" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F155" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G155" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H155" t="s">
+        <v>0</v>
+      </c>
+      <c r="I155" t="s">
+        <v>161</v>
+      </c>
+      <c r="J155" t="s">
+        <v>0</v>
+      </c>
+      <c r="K155" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L155" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>173</v>
+      </c>
+      <c r="B156" t="s">
+        <v>0</v>
+      </c>
+      <c r="C156" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D156" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E156" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F156" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G156" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H156" t="s">
+        <v>0</v>
+      </c>
+      <c r="I156" t="s">
+        <v>161</v>
+      </c>
+      <c r="J156" t="s">
+        <v>0</v>
+      </c>
+      <c r="K156" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L156" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>174</v>
+      </c>
+      <c r="B157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D157" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E157" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F157" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G157" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H157" t="s">
+        <v>0</v>
+      </c>
+      <c r="I157" t="s">
+        <v>161</v>
+      </c>
+      <c r="J157" t="s">
+        <v>0</v>
+      </c>
+      <c r="K157" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L157" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>175</v>
+      </c>
+      <c r="B158" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D158" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E158" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F158" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G158" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H158" t="s">
+        <v>0</v>
+      </c>
+      <c r="I158" t="s">
+        <v>161</v>
+      </c>
+      <c r="J158" t="s">
+        <v>0</v>
+      </c>
+      <c r="K158" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L158" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>176</v>
+      </c>
+      <c r="B159" t="s">
+        <v>0</v>
+      </c>
+      <c r="C159" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D159" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E159" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F159" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G159" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H159" t="s">
+        <v>0</v>
+      </c>
+      <c r="I159" t="s">
+        <v>161</v>
+      </c>
+      <c r="J159" t="s">
+        <v>0</v>
+      </c>
+      <c r="K159" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L159" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>177</v>
+      </c>
+      <c r="B160" t="s">
+        <v>0</v>
+      </c>
+      <c r="C160" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D160" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E160" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F160" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G160" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H160" t="s">
+        <v>0</v>
+      </c>
+      <c r="I160" t="s">
+        <v>161</v>
+      </c>
+      <c r="J160" t="s">
+        <v>0</v>
+      </c>
+      <c r="K160" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L160" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>178</v>
+      </c>
+      <c r="B161" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D161" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E161" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F161" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G161" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H161" t="s">
+        <v>0</v>
+      </c>
+      <c r="I161" t="s">
+        <v>161</v>
+      </c>
+      <c r="J161" t="s">
+        <v>0</v>
+      </c>
+      <c r="K161" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L161" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>179</v>
+      </c>
+      <c r="B162" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D162" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E162" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F162" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G162" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H162" t="s">
+        <v>0</v>
+      </c>
+      <c r="I162" t="s">
+        <v>161</v>
+      </c>
+      <c r="J162" t="s">
+        <v>0</v>
+      </c>
+      <c r="K162" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L162" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10043,7 +11319,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H427"/>
+  <dimension ref="A1:H484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -21156,6 +22432,1488 @@
         <v>8193.0</v>
       </c>
     </row>
+    <row r="428">
+      <c r="A428" t="s">
+        <v>160</v>
+      </c>
+      <c r="B428" t="s">
+        <v>0</v>
+      </c>
+      <c r="C428" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D428" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E428" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F428" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G428" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H428" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="s">
+        <v>160</v>
+      </c>
+      <c r="B429" t="s">
+        <v>0</v>
+      </c>
+      <c r="C429" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D429" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E429" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F429" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G429" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H429" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="s">
+        <v>160</v>
+      </c>
+      <c r="B430" t="s">
+        <v>0</v>
+      </c>
+      <c r="C430" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D430" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E430" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F430" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G430" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H430" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="s">
+        <v>162</v>
+      </c>
+      <c r="B431" t="s">
+        <v>0</v>
+      </c>
+      <c r="C431" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D431" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E431" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F431" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G431" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H431" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="s">
+        <v>162</v>
+      </c>
+      <c r="B432" t="s">
+        <v>0</v>
+      </c>
+      <c r="C432" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D432" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E432" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F432" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G432" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H432" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="s">
+        <v>162</v>
+      </c>
+      <c r="B433" t="s">
+        <v>0</v>
+      </c>
+      <c r="C433" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D433" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E433" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F433" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G433" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H433" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="s">
+        <v>163</v>
+      </c>
+      <c r="B434" t="s">
+        <v>0</v>
+      </c>
+      <c r="C434" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D434" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E434" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F434" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G434" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H434" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="s">
+        <v>163</v>
+      </c>
+      <c r="B435" t="s">
+        <v>0</v>
+      </c>
+      <c r="C435" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D435" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E435" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F435" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G435" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H435" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="s">
+        <v>163</v>
+      </c>
+      <c r="B436" t="s">
+        <v>0</v>
+      </c>
+      <c r="C436" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D436" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E436" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F436" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G436" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H436" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="s">
+        <v>164</v>
+      </c>
+      <c r="B437" t="s">
+        <v>0</v>
+      </c>
+      <c r="C437" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D437" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E437" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F437" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G437" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H437" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="s">
+        <v>164</v>
+      </c>
+      <c r="B438" t="s">
+        <v>0</v>
+      </c>
+      <c r="C438" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D438" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E438" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F438" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G438" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H438" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="s">
+        <v>164</v>
+      </c>
+      <c r="B439" t="s">
+        <v>0</v>
+      </c>
+      <c r="C439" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D439" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E439" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F439" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G439" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H439" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="s">
+        <v>165</v>
+      </c>
+      <c r="B440" t="s">
+        <v>0</v>
+      </c>
+      <c r="C440" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D440" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E440" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F440" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G440" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H440" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="s">
+        <v>165</v>
+      </c>
+      <c r="B441" t="s">
+        <v>0</v>
+      </c>
+      <c r="C441" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D441" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E441" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F441" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G441" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H441" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="s">
+        <v>165</v>
+      </c>
+      <c r="B442" t="s">
+        <v>0</v>
+      </c>
+      <c r="C442" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D442" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E442" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F442" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G442" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H442" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="s">
+        <v>166</v>
+      </c>
+      <c r="B443" t="s">
+        <v>0</v>
+      </c>
+      <c r="C443" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D443" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E443" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F443" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G443" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H443" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="s">
+        <v>166</v>
+      </c>
+      <c r="B444" t="s">
+        <v>0</v>
+      </c>
+      <c r="C444" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D444" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E444" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F444" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G444" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H444" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="s">
+        <v>166</v>
+      </c>
+      <c r="B445" t="s">
+        <v>0</v>
+      </c>
+      <c r="C445" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D445" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E445" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F445" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G445" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H445" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="s">
+        <v>167</v>
+      </c>
+      <c r="B446" t="s">
+        <v>0</v>
+      </c>
+      <c r="C446" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D446" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E446" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F446" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G446" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H446" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="s">
+        <v>167</v>
+      </c>
+      <c r="B447" t="s">
+        <v>0</v>
+      </c>
+      <c r="C447" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D447" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E447" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F447" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G447" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H447" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="s">
+        <v>167</v>
+      </c>
+      <c r="B448" t="s">
+        <v>0</v>
+      </c>
+      <c r="C448" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D448" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E448" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F448" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G448" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H448" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="s">
+        <v>168</v>
+      </c>
+      <c r="B449" t="s">
+        <v>0</v>
+      </c>
+      <c r="C449" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D449" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E449" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F449" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G449" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H449" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="s">
+        <v>168</v>
+      </c>
+      <c r="B450" t="s">
+        <v>0</v>
+      </c>
+      <c r="C450" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D450" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E450" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F450" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G450" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H450" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="s">
+        <v>168</v>
+      </c>
+      <c r="B451" t="s">
+        <v>0</v>
+      </c>
+      <c r="C451" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D451" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E451" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F451" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G451" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H451" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="s">
+        <v>169</v>
+      </c>
+      <c r="B452" t="s">
+        <v>0</v>
+      </c>
+      <c r="C452" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D452" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E452" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F452" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G452" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H452" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="s">
+        <v>169</v>
+      </c>
+      <c r="B453" t="s">
+        <v>0</v>
+      </c>
+      <c r="C453" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D453" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E453" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F453" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G453" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H453" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="s">
+        <v>169</v>
+      </c>
+      <c r="B454" t="s">
+        <v>0</v>
+      </c>
+      <c r="C454" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D454" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E454" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F454" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G454" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H454" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="s">
+        <v>170</v>
+      </c>
+      <c r="B455" t="s">
+        <v>0</v>
+      </c>
+      <c r="C455" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D455" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E455" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F455" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G455" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H455" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="s">
+        <v>170</v>
+      </c>
+      <c r="B456" t="s">
+        <v>0</v>
+      </c>
+      <c r="C456" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D456" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E456" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F456" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G456" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H456" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="s">
+        <v>170</v>
+      </c>
+      <c r="B457" t="s">
+        <v>0</v>
+      </c>
+      <c r="C457" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D457" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E457" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F457" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G457" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H457" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="s">
+        <v>171</v>
+      </c>
+      <c r="B458" t="s">
+        <v>0</v>
+      </c>
+      <c r="C458" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D458" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E458" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F458" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G458" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H458" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="s">
+        <v>171</v>
+      </c>
+      <c r="B459" t="s">
+        <v>0</v>
+      </c>
+      <c r="C459" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D459" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E459" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F459" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G459" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H459" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="s">
+        <v>171</v>
+      </c>
+      <c r="B460" t="s">
+        <v>0</v>
+      </c>
+      <c r="C460" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D460" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E460" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F460" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G460" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H460" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="s">
+        <v>172</v>
+      </c>
+      <c r="B461" t="s">
+        <v>0</v>
+      </c>
+      <c r="C461" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D461" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E461" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F461" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G461" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H461" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="s">
+        <v>172</v>
+      </c>
+      <c r="B462" t="s">
+        <v>0</v>
+      </c>
+      <c r="C462" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D462" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E462" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F462" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G462" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H462" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="s">
+        <v>172</v>
+      </c>
+      <c r="B463" t="s">
+        <v>0</v>
+      </c>
+      <c r="C463" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D463" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E463" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F463" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G463" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H463" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="s">
+        <v>173</v>
+      </c>
+      <c r="B464" t="s">
+        <v>0</v>
+      </c>
+      <c r="C464" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D464" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E464" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F464" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G464" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H464" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="s">
+        <v>173</v>
+      </c>
+      <c r="B465" t="s">
+        <v>0</v>
+      </c>
+      <c r="C465" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D465" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E465" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F465" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G465" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H465" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="s">
+        <v>173</v>
+      </c>
+      <c r="B466" t="s">
+        <v>0</v>
+      </c>
+      <c r="C466" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D466" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E466" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F466" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G466" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H466" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="s">
+        <v>174</v>
+      </c>
+      <c r="B467" t="s">
+        <v>0</v>
+      </c>
+      <c r="C467" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D467" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E467" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F467" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G467" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H467" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="s">
+        <v>174</v>
+      </c>
+      <c r="B468" t="s">
+        <v>0</v>
+      </c>
+      <c r="C468" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D468" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E468" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F468" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G468" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H468" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="s">
+        <v>174</v>
+      </c>
+      <c r="B469" t="s">
+        <v>0</v>
+      </c>
+      <c r="C469" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D469" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E469" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F469" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G469" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H469" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="s">
+        <v>175</v>
+      </c>
+      <c r="B470" t="s">
+        <v>0</v>
+      </c>
+      <c r="C470" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D470" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E470" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F470" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G470" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H470" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="s">
+        <v>175</v>
+      </c>
+      <c r="B471" t="s">
+        <v>0</v>
+      </c>
+      <c r="C471" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D471" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E471" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F471" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G471" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H471" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="s">
+        <v>175</v>
+      </c>
+      <c r="B472" t="s">
+        <v>0</v>
+      </c>
+      <c r="C472" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D472" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E472" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F472" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G472" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H472" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="s">
+        <v>176</v>
+      </c>
+      <c r="B473" t="s">
+        <v>0</v>
+      </c>
+      <c r="C473" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D473" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E473" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F473" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G473" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H473" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="s">
+        <v>176</v>
+      </c>
+      <c r="B474" t="s">
+        <v>0</v>
+      </c>
+      <c r="C474" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D474" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E474" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F474" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G474" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H474" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="s">
+        <v>176</v>
+      </c>
+      <c r="B475" t="s">
+        <v>0</v>
+      </c>
+      <c r="C475" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D475" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E475" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F475" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G475" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H475" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="s">
+        <v>177</v>
+      </c>
+      <c r="B476" t="s">
+        <v>0</v>
+      </c>
+      <c r="C476" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D476" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E476" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F476" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G476" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H476" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="s">
+        <v>177</v>
+      </c>
+      <c r="B477" t="s">
+        <v>0</v>
+      </c>
+      <c r="C477" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D477" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E477" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F477" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G477" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H477" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="s">
+        <v>177</v>
+      </c>
+      <c r="B478" t="s">
+        <v>0</v>
+      </c>
+      <c r="C478" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D478" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E478" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F478" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G478" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H478" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="s">
+        <v>178</v>
+      </c>
+      <c r="B479" t="s">
+        <v>0</v>
+      </c>
+      <c r="C479" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D479" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E479" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F479" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G479" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H479" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="s">
+        <v>178</v>
+      </c>
+      <c r="B480" t="s">
+        <v>0</v>
+      </c>
+      <c r="C480" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D480" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E480" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F480" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G480" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H480" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="s">
+        <v>178</v>
+      </c>
+      <c r="B481" t="s">
+        <v>0</v>
+      </c>
+      <c r="C481" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D481" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E481" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F481" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G481" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H481" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="s">
+        <v>179</v>
+      </c>
+      <c r="B482" t="s">
+        <v>0</v>
+      </c>
+      <c r="C482" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D482" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E482" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F482" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G482" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H482" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="s">
+        <v>179</v>
+      </c>
+      <c r="B483" t="s">
+        <v>0</v>
+      </c>
+      <c r="C483" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D483" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E483" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F483" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G483" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H483" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="s">
+        <v>179</v>
+      </c>
+      <c r="B484" t="s">
+        <v>0</v>
+      </c>
+      <c r="C484" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D484" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E484" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F484" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G484" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H484" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- automatic reconnection on connection lost
</commit_message>
<xml_diff>
--- a/data/sheet/msg_8705.xlsx
+++ b/data/sheet/msg_8705.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4903" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5563" uniqueCount="204">
   <si>
     <t/>
   </si>
@@ -569,6 +569,72 @@
   <si>
     <t>2022-03-22 20:21:31</t>
   </si>
+  <si>
+    <t>2022-03-25 13:47:48</t>
+  </si>
+  <si>
+    <t>2022-03-25 14:00:50</t>
+  </si>
+  <si>
+    <t>2022-03-25 14:04:52</t>
+  </si>
+  <si>
+    <t>2022-03-25 14:13:55</t>
+  </si>
+  <si>
+    <t>2022-06-09 13:48:08</t>
+  </si>
+  <si>
+    <t>2022-06-09 16:48:29</t>
+  </si>
+  <si>
+    <t>2022-06-09 19:06:45</t>
+  </si>
+  <si>
+    <t>2022-06-09 22:55:57</t>
+  </si>
+  <si>
+    <t>2022-06-10 09:18:11</t>
+  </si>
+  <si>
+    <t>2022-06-10 13:52:02</t>
+  </si>
+  <si>
+    <t>2022-06-10 16:30:16</t>
+  </si>
+  <si>
+    <t>2022-06-10 18:50:26</t>
+  </si>
+  <si>
+    <t>2022-06-11 08:02:11</t>
+  </si>
+  <si>
+    <t>2022-06-24 12:59:38</t>
+  </si>
+  <si>
+    <t>2022-06-25 00:36:26</t>
+  </si>
+  <si>
+    <t>2022-06-25 06:32:08</t>
+  </si>
+  <si>
+    <t>2022-06-25 11:08:34</t>
+  </si>
+  <si>
+    <t>2022-06-25 12:40:03</t>
+  </si>
+  <si>
+    <t>2022-06-25 13:03:06</t>
+  </si>
+  <si>
+    <t>2022-07-01 16:36:25</t>
+  </si>
+  <si>
+    <t>2022-07-01 17:16:32</t>
+  </si>
+  <si>
+    <t>2022-07-01 17:40:35</t>
+  </si>
 </sst>
 </file>
 
@@ -920,7 +986,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H164"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5195,6 +5261,578 @@
         <v>255.0</v>
       </c>
     </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>182</v>
+      </c>
+      <c r="B165" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165" t="s">
+        <v>10</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1.64821247E9</v>
+      </c>
+      <c r="E165" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F165" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G165" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H165" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>183</v>
+      </c>
+      <c r="B166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C166" t="s">
+        <v>10</v>
+      </c>
+      <c r="D166" t="n">
+        <v>1.648213252E9</v>
+      </c>
+      <c r="E166" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F166" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G166" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H166" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>184</v>
+      </c>
+      <c r="B167" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167" t="s">
+        <v>10</v>
+      </c>
+      <c r="D167" t="n">
+        <v>1.648213495E9</v>
+      </c>
+      <c r="E167" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F167" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G167" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H167" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>185</v>
+      </c>
+      <c r="B168" t="s">
+        <v>0</v>
+      </c>
+      <c r="C168" t="s">
+        <v>10</v>
+      </c>
+      <c r="D168" t="n">
+        <v>1.648214037E9</v>
+      </c>
+      <c r="E168" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F168" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G168" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H168" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>186</v>
+      </c>
+      <c r="B169" t="s">
+        <v>0</v>
+      </c>
+      <c r="C169" t="s">
+        <v>10</v>
+      </c>
+      <c r="D169" t="n">
+        <v>1.654775301E9</v>
+      </c>
+      <c r="E169" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F169" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G169" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H169" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>187</v>
+      </c>
+      <c r="B170" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170" t="s">
+        <v>10</v>
+      </c>
+      <c r="D170" t="n">
+        <v>1.654786123E9</v>
+      </c>
+      <c r="E170" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F170" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G170" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H170" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>188</v>
+      </c>
+      <c r="B171" t="s">
+        <v>0</v>
+      </c>
+      <c r="C171" t="s">
+        <v>10</v>
+      </c>
+      <c r="D171" t="n">
+        <v>1.654794419E9</v>
+      </c>
+      <c r="E171" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F171" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G171" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H171" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>189</v>
+      </c>
+      <c r="B172" t="s">
+        <v>0</v>
+      </c>
+      <c r="C172" t="s">
+        <v>10</v>
+      </c>
+      <c r="D172" t="n">
+        <v>1.654808173E9</v>
+      </c>
+      <c r="E172" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F172" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G172" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H172" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>190</v>
+      </c>
+      <c r="B173" t="s">
+        <v>0</v>
+      </c>
+      <c r="C173" t="s">
+        <v>10</v>
+      </c>
+      <c r="D173" t="n">
+        <v>1.654845492E9</v>
+      </c>
+      <c r="E173" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F173" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G173" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H173" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>191</v>
+      </c>
+      <c r="B174" t="s">
+        <v>0</v>
+      </c>
+      <c r="C174" t="s">
+        <v>10</v>
+      </c>
+      <c r="D174" t="n">
+        <v>1.654861924E9</v>
+      </c>
+      <c r="E174" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F174" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G174" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H174" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>192</v>
+      </c>
+      <c r="B175" t="s">
+        <v>0</v>
+      </c>
+      <c r="C175" t="s">
+        <v>10</v>
+      </c>
+      <c r="D175" t="n">
+        <v>1.654871419E9</v>
+      </c>
+      <c r="E175" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F175" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G175" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H175" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>193</v>
+      </c>
+      <c r="B176" t="s">
+        <v>0</v>
+      </c>
+      <c r="C176" t="s">
+        <v>10</v>
+      </c>
+      <c r="D176" t="n">
+        <v>1.654879829E9</v>
+      </c>
+      <c r="E176" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F176" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G176" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H176" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>194</v>
+      </c>
+      <c r="B177" t="s">
+        <v>0</v>
+      </c>
+      <c r="C177" t="s">
+        <v>10</v>
+      </c>
+      <c r="D177" t="n">
+        <v>1.654927337E9</v>
+      </c>
+      <c r="E177" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F177" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G177" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H177" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>195</v>
+      </c>
+      <c r="B178" t="s">
+        <v>0</v>
+      </c>
+      <c r="C178" t="s">
+        <v>10</v>
+      </c>
+      <c r="D178" t="n">
+        <v>1.656068379E9</v>
+      </c>
+      <c r="E178" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F178" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G178" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H178" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>196</v>
+      </c>
+      <c r="B179" t="s">
+        <v>0</v>
+      </c>
+      <c r="C179" t="s">
+        <v>10</v>
+      </c>
+      <c r="D179" t="n">
+        <v>1.65611019E9</v>
+      </c>
+      <c r="E179" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F179" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G179" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H179" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>197</v>
+      </c>
+      <c r="B180" t="s">
+        <v>0</v>
+      </c>
+      <c r="C180" t="s">
+        <v>10</v>
+      </c>
+      <c r="D180" t="n">
+        <v>1.656131526E9</v>
+      </c>
+      <c r="E180" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F180" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G180" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H180" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>198</v>
+      </c>
+      <c r="B181" t="s">
+        <v>0</v>
+      </c>
+      <c r="C181" t="s">
+        <v>10</v>
+      </c>
+      <c r="D181" t="n">
+        <v>1.656148113E9</v>
+      </c>
+      <c r="E181" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F181" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G181" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H181" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>199</v>
+      </c>
+      <c r="B182" t="s">
+        <v>0</v>
+      </c>
+      <c r="C182" t="s">
+        <v>10</v>
+      </c>
+      <c r="D182" t="n">
+        <v>1.656153603E9</v>
+      </c>
+      <c r="E182" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F182" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G182" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H182" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>200</v>
+      </c>
+      <c r="B183" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183" t="n">
+        <v>1.656154987E9</v>
+      </c>
+      <c r="E183" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F183" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G183" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H183" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>201</v>
+      </c>
+      <c r="B184" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" t="s">
+        <v>10</v>
+      </c>
+      <c r="D184" t="n">
+        <v>1.656686193E9</v>
+      </c>
+      <c r="E184" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F184" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G184" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H184" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>202</v>
+      </c>
+      <c r="B185" t="s">
+        <v>0</v>
+      </c>
+      <c r="C185" t="s">
+        <v>10</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1.656688601E9</v>
+      </c>
+      <c r="E185" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F185" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G185" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H185" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>203</v>
+      </c>
+      <c r="B186" t="s">
+        <v>0</v>
+      </c>
+      <c r="C186" t="s">
+        <v>10</v>
+      </c>
+      <c r="D186" t="n">
+        <v>1.656690043E9</v>
+      </c>
+      <c r="E186" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F186" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="G186" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H186" t="n">
+        <v>255.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5202,7 +5840,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L164"/>
+  <dimension ref="A1:L186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -11446,6 +12084,842 @@
         <v>0</v>
       </c>
     </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>182</v>
+      </c>
+      <c r="B165" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D165" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E165" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F165" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G165" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H165" t="s">
+        <v>0</v>
+      </c>
+      <c r="I165" t="s">
+        <v>161</v>
+      </c>
+      <c r="J165" t="s">
+        <v>0</v>
+      </c>
+      <c r="K165" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L165" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>183</v>
+      </c>
+      <c r="B166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C166" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D166" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E166" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F166" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G166" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H166" t="s">
+        <v>0</v>
+      </c>
+      <c r="I166" t="s">
+        <v>161</v>
+      </c>
+      <c r="J166" t="s">
+        <v>0</v>
+      </c>
+      <c r="K166" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L166" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>184</v>
+      </c>
+      <c r="B167" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D167" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E167" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F167" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G167" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H167" t="s">
+        <v>0</v>
+      </c>
+      <c r="I167" t="s">
+        <v>161</v>
+      </c>
+      <c r="J167" t="s">
+        <v>0</v>
+      </c>
+      <c r="K167" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L167" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>185</v>
+      </c>
+      <c r="B168" t="s">
+        <v>0</v>
+      </c>
+      <c r="C168" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D168" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E168" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F168" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G168" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H168" t="s">
+        <v>0</v>
+      </c>
+      <c r="I168" t="s">
+        <v>161</v>
+      </c>
+      <c r="J168" t="s">
+        <v>0</v>
+      </c>
+      <c r="K168" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L168" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>186</v>
+      </c>
+      <c r="B169" t="s">
+        <v>0</v>
+      </c>
+      <c r="C169" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D169" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E169" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F169" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G169" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H169" t="s">
+        <v>0</v>
+      </c>
+      <c r="I169" t="s">
+        <v>161</v>
+      </c>
+      <c r="J169" t="s">
+        <v>0</v>
+      </c>
+      <c r="K169" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L169" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>187</v>
+      </c>
+      <c r="B170" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D170" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E170" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F170" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G170" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H170" t="s">
+        <v>0</v>
+      </c>
+      <c r="I170" t="s">
+        <v>161</v>
+      </c>
+      <c r="J170" t="s">
+        <v>0</v>
+      </c>
+      <c r="K170" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L170" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>188</v>
+      </c>
+      <c r="B171" t="s">
+        <v>0</v>
+      </c>
+      <c r="C171" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D171" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E171" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F171" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G171" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H171" t="s">
+        <v>0</v>
+      </c>
+      <c r="I171" t="s">
+        <v>161</v>
+      </c>
+      <c r="J171" t="s">
+        <v>0</v>
+      </c>
+      <c r="K171" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L171" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>189</v>
+      </c>
+      <c r="B172" t="s">
+        <v>0</v>
+      </c>
+      <c r="C172" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D172" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E172" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F172" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G172" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H172" t="s">
+        <v>0</v>
+      </c>
+      <c r="I172" t="s">
+        <v>161</v>
+      </c>
+      <c r="J172" t="s">
+        <v>0</v>
+      </c>
+      <c r="K172" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L172" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>190</v>
+      </c>
+      <c r="B173" t="s">
+        <v>0</v>
+      </c>
+      <c r="C173" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D173" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E173" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F173" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G173" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H173" t="s">
+        <v>0</v>
+      </c>
+      <c r="I173" t="s">
+        <v>161</v>
+      </c>
+      <c r="J173" t="s">
+        <v>0</v>
+      </c>
+      <c r="K173" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L173" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>191</v>
+      </c>
+      <c r="B174" t="s">
+        <v>0</v>
+      </c>
+      <c r="C174" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D174" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E174" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F174" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G174" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H174" t="s">
+        <v>0</v>
+      </c>
+      <c r="I174" t="s">
+        <v>161</v>
+      </c>
+      <c r="J174" t="s">
+        <v>0</v>
+      </c>
+      <c r="K174" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L174" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>192</v>
+      </c>
+      <c r="B175" t="s">
+        <v>0</v>
+      </c>
+      <c r="C175" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D175" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E175" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F175" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G175" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H175" t="s">
+        <v>0</v>
+      </c>
+      <c r="I175" t="s">
+        <v>161</v>
+      </c>
+      <c r="J175" t="s">
+        <v>0</v>
+      </c>
+      <c r="K175" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L175" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>193</v>
+      </c>
+      <c r="B176" t="s">
+        <v>0</v>
+      </c>
+      <c r="C176" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D176" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E176" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F176" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G176" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H176" t="s">
+        <v>0</v>
+      </c>
+      <c r="I176" t="s">
+        <v>161</v>
+      </c>
+      <c r="J176" t="s">
+        <v>0</v>
+      </c>
+      <c r="K176" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L176" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>194</v>
+      </c>
+      <c r="B177" t="s">
+        <v>0</v>
+      </c>
+      <c r="C177" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D177" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E177" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F177" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G177" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H177" t="s">
+        <v>0</v>
+      </c>
+      <c r="I177" t="s">
+        <v>161</v>
+      </c>
+      <c r="J177" t="s">
+        <v>0</v>
+      </c>
+      <c r="K177" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L177" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>195</v>
+      </c>
+      <c r="B178" t="s">
+        <v>0</v>
+      </c>
+      <c r="C178" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D178" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E178" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F178" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G178" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H178" t="s">
+        <v>0</v>
+      </c>
+      <c r="I178" t="s">
+        <v>161</v>
+      </c>
+      <c r="J178" t="s">
+        <v>0</v>
+      </c>
+      <c r="K178" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L178" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>196</v>
+      </c>
+      <c r="B179" t="s">
+        <v>0</v>
+      </c>
+      <c r="C179" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D179" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E179" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F179" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G179" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H179" t="s">
+        <v>0</v>
+      </c>
+      <c r="I179" t="s">
+        <v>161</v>
+      </c>
+      <c r="J179" t="s">
+        <v>0</v>
+      </c>
+      <c r="K179" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L179" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>197</v>
+      </c>
+      <c r="B180" t="s">
+        <v>0</v>
+      </c>
+      <c r="C180" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D180" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E180" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F180" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G180" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H180" t="s">
+        <v>0</v>
+      </c>
+      <c r="I180" t="s">
+        <v>161</v>
+      </c>
+      <c r="J180" t="s">
+        <v>0</v>
+      </c>
+      <c r="K180" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L180" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>198</v>
+      </c>
+      <c r="B181" t="s">
+        <v>0</v>
+      </c>
+      <c r="C181" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D181" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E181" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F181" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G181" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H181" t="s">
+        <v>0</v>
+      </c>
+      <c r="I181" t="s">
+        <v>161</v>
+      </c>
+      <c r="J181" t="s">
+        <v>0</v>
+      </c>
+      <c r="K181" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L181" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>199</v>
+      </c>
+      <c r="B182" t="s">
+        <v>0</v>
+      </c>
+      <c r="C182" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D182" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E182" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F182" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G182" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H182" t="s">
+        <v>0</v>
+      </c>
+      <c r="I182" t="s">
+        <v>161</v>
+      </c>
+      <c r="J182" t="s">
+        <v>0</v>
+      </c>
+      <c r="K182" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L182" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>200</v>
+      </c>
+      <c r="B183" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D183" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E183" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F183" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G183" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H183" t="s">
+        <v>0</v>
+      </c>
+      <c r="I183" t="s">
+        <v>161</v>
+      </c>
+      <c r="J183" t="s">
+        <v>0</v>
+      </c>
+      <c r="K183" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L183" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>201</v>
+      </c>
+      <c r="B184" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D184" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E184" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F184" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G184" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H184" t="s">
+        <v>0</v>
+      </c>
+      <c r="I184" t="s">
+        <v>161</v>
+      </c>
+      <c r="J184" t="s">
+        <v>0</v>
+      </c>
+      <c r="K184" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L184" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>202</v>
+      </c>
+      <c r="B185" t="s">
+        <v>0</v>
+      </c>
+      <c r="C185" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D185" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E185" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F185" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G185" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H185" t="s">
+        <v>0</v>
+      </c>
+      <c r="I185" t="s">
+        <v>161</v>
+      </c>
+      <c r="J185" t="s">
+        <v>0</v>
+      </c>
+      <c r="K185" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L185" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>203</v>
+      </c>
+      <c r="B186" t="s">
+        <v>0</v>
+      </c>
+      <c r="C186" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="D186" t="n">
+        <v>37122.0</v>
+      </c>
+      <c r="E186" t="n">
+        <v>655618.0</v>
+      </c>
+      <c r="F186" t="n">
+        <v>1.0485764E7</v>
+      </c>
+      <c r="G186" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H186" t="s">
+        <v>0</v>
+      </c>
+      <c r="I186" t="s">
+        <v>161</v>
+      </c>
+      <c r="J186" t="s">
+        <v>0</v>
+      </c>
+      <c r="K186" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L186" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11453,7 +12927,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H490"/>
+  <dimension ref="A1:H556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -24204,6 +25678,1722 @@
         <v>8193.0</v>
       </c>
     </row>
+    <row r="491">
+      <c r="A491" t="s">
+        <v>182</v>
+      </c>
+      <c r="B491" t="s">
+        <v>0</v>
+      </c>
+      <c r="C491" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D491" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E491" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F491" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G491" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H491" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="s">
+        <v>182</v>
+      </c>
+      <c r="B492" t="s">
+        <v>0</v>
+      </c>
+      <c r="C492" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D492" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E492" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F492" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G492" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H492" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="s">
+        <v>182</v>
+      </c>
+      <c r="B493" t="s">
+        <v>0</v>
+      </c>
+      <c r="C493" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D493" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E493" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F493" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G493" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H493" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="s">
+        <v>183</v>
+      </c>
+      <c r="B494" t="s">
+        <v>0</v>
+      </c>
+      <c r="C494" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D494" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E494" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F494" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G494" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H494" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="s">
+        <v>183</v>
+      </c>
+      <c r="B495" t="s">
+        <v>0</v>
+      </c>
+      <c r="C495" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D495" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E495" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F495" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G495" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H495" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="s">
+        <v>183</v>
+      </c>
+      <c r="B496" t="s">
+        <v>0</v>
+      </c>
+      <c r="C496" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D496" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E496" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F496" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G496" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H496" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="s">
+        <v>184</v>
+      </c>
+      <c r="B497" t="s">
+        <v>0</v>
+      </c>
+      <c r="C497" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D497" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E497" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F497" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G497" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H497" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="s">
+        <v>184</v>
+      </c>
+      <c r="B498" t="s">
+        <v>0</v>
+      </c>
+      <c r="C498" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D498" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E498" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F498" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G498" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H498" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="s">
+        <v>184</v>
+      </c>
+      <c r="B499" t="s">
+        <v>0</v>
+      </c>
+      <c r="C499" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D499" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E499" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F499" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G499" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H499" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="s">
+        <v>185</v>
+      </c>
+      <c r="B500" t="s">
+        <v>0</v>
+      </c>
+      <c r="C500" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D500" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E500" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F500" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G500" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H500" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="s">
+        <v>185</v>
+      </c>
+      <c r="B501" t="s">
+        <v>0</v>
+      </c>
+      <c r="C501" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D501" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E501" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F501" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G501" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H501" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="s">
+        <v>185</v>
+      </c>
+      <c r="B502" t="s">
+        <v>0</v>
+      </c>
+      <c r="C502" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D502" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E502" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F502" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G502" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H502" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="s">
+        <v>186</v>
+      </c>
+      <c r="B503" t="s">
+        <v>0</v>
+      </c>
+      <c r="C503" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D503" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E503" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F503" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G503" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H503" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="s">
+        <v>186</v>
+      </c>
+      <c r="B504" t="s">
+        <v>0</v>
+      </c>
+      <c r="C504" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D504" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E504" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F504" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G504" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H504" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="s">
+        <v>186</v>
+      </c>
+      <c r="B505" t="s">
+        <v>0</v>
+      </c>
+      <c r="C505" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D505" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E505" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F505" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G505" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H505" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="s">
+        <v>187</v>
+      </c>
+      <c r="B506" t="s">
+        <v>0</v>
+      </c>
+      <c r="C506" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D506" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E506" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F506" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G506" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H506" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="s">
+        <v>187</v>
+      </c>
+      <c r="B507" t="s">
+        <v>0</v>
+      </c>
+      <c r="C507" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D507" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E507" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F507" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G507" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H507" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="s">
+        <v>187</v>
+      </c>
+      <c r="B508" t="s">
+        <v>0</v>
+      </c>
+      <c r="C508" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D508" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E508" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F508" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G508" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H508" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="s">
+        <v>188</v>
+      </c>
+      <c r="B509" t="s">
+        <v>0</v>
+      </c>
+      <c r="C509" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D509" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E509" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F509" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G509" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H509" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="s">
+        <v>188</v>
+      </c>
+      <c r="B510" t="s">
+        <v>0</v>
+      </c>
+      <c r="C510" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D510" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E510" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F510" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G510" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H510" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="s">
+        <v>188</v>
+      </c>
+      <c r="B511" t="s">
+        <v>0</v>
+      </c>
+      <c r="C511" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D511" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E511" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F511" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G511" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H511" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="s">
+        <v>189</v>
+      </c>
+      <c r="B512" t="s">
+        <v>0</v>
+      </c>
+      <c r="C512" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D512" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E512" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F512" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G512" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H512" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="s">
+        <v>189</v>
+      </c>
+      <c r="B513" t="s">
+        <v>0</v>
+      </c>
+      <c r="C513" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D513" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E513" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F513" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G513" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H513" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="s">
+        <v>189</v>
+      </c>
+      <c r="B514" t="s">
+        <v>0</v>
+      </c>
+      <c r="C514" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D514" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E514" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F514" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G514" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H514" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="s">
+        <v>190</v>
+      </c>
+      <c r="B515" t="s">
+        <v>0</v>
+      </c>
+      <c r="C515" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D515" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E515" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F515" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G515" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H515" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="s">
+        <v>190</v>
+      </c>
+      <c r="B516" t="s">
+        <v>0</v>
+      </c>
+      <c r="C516" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D516" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E516" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F516" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G516" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H516" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="s">
+        <v>190</v>
+      </c>
+      <c r="B517" t="s">
+        <v>0</v>
+      </c>
+      <c r="C517" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D517" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E517" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F517" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G517" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H517" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="s">
+        <v>191</v>
+      </c>
+      <c r="B518" t="s">
+        <v>0</v>
+      </c>
+      <c r="C518" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D518" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E518" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F518" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G518" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H518" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="s">
+        <v>191</v>
+      </c>
+      <c r="B519" t="s">
+        <v>0</v>
+      </c>
+      <c r="C519" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D519" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E519" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F519" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G519" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H519" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="s">
+        <v>191</v>
+      </c>
+      <c r="B520" t="s">
+        <v>0</v>
+      </c>
+      <c r="C520" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D520" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E520" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F520" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G520" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H520" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="s">
+        <v>192</v>
+      </c>
+      <c r="B521" t="s">
+        <v>0</v>
+      </c>
+      <c r="C521" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D521" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E521" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F521" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G521" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H521" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="s">
+        <v>192</v>
+      </c>
+      <c r="B522" t="s">
+        <v>0</v>
+      </c>
+      <c r="C522" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D522" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E522" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F522" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G522" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H522" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="s">
+        <v>192</v>
+      </c>
+      <c r="B523" t="s">
+        <v>0</v>
+      </c>
+      <c r="C523" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D523" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E523" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F523" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G523" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H523" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="s">
+        <v>193</v>
+      </c>
+      <c r="B524" t="s">
+        <v>0</v>
+      </c>
+      <c r="C524" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D524" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E524" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F524" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G524" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H524" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="s">
+        <v>193</v>
+      </c>
+      <c r="B525" t="s">
+        <v>0</v>
+      </c>
+      <c r="C525" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D525" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E525" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F525" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G525" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H525" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="s">
+        <v>193</v>
+      </c>
+      <c r="B526" t="s">
+        <v>0</v>
+      </c>
+      <c r="C526" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D526" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E526" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F526" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G526" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H526" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="s">
+        <v>194</v>
+      </c>
+      <c r="B527" t="s">
+        <v>0</v>
+      </c>
+      <c r="C527" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D527" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E527" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F527" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G527" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H527" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="s">
+        <v>194</v>
+      </c>
+      <c r="B528" t="s">
+        <v>0</v>
+      </c>
+      <c r="C528" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D528" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E528" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F528" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G528" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H528" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="s">
+        <v>194</v>
+      </c>
+      <c r="B529" t="s">
+        <v>0</v>
+      </c>
+      <c r="C529" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D529" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E529" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F529" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G529" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H529" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="s">
+        <v>195</v>
+      </c>
+      <c r="B530" t="s">
+        <v>0</v>
+      </c>
+      <c r="C530" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D530" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E530" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F530" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G530" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H530" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="s">
+        <v>195</v>
+      </c>
+      <c r="B531" t="s">
+        <v>0</v>
+      </c>
+      <c r="C531" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D531" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E531" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F531" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G531" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H531" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="s">
+        <v>195</v>
+      </c>
+      <c r="B532" t="s">
+        <v>0</v>
+      </c>
+      <c r="C532" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D532" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E532" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F532" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G532" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H532" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="s">
+        <v>196</v>
+      </c>
+      <c r="B533" t="s">
+        <v>0</v>
+      </c>
+      <c r="C533" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D533" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E533" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F533" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G533" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H533" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="s">
+        <v>196</v>
+      </c>
+      <c r="B534" t="s">
+        <v>0</v>
+      </c>
+      <c r="C534" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D534" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E534" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F534" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G534" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H534" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="s">
+        <v>196</v>
+      </c>
+      <c r="B535" t="s">
+        <v>0</v>
+      </c>
+      <c r="C535" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D535" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E535" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F535" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G535" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H535" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="s">
+        <v>197</v>
+      </c>
+      <c r="B536" t="s">
+        <v>0</v>
+      </c>
+      <c r="C536" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D536" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E536" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F536" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G536" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H536" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="s">
+        <v>197</v>
+      </c>
+      <c r="B537" t="s">
+        <v>0</v>
+      </c>
+      <c r="C537" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D537" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E537" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F537" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G537" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H537" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="s">
+        <v>197</v>
+      </c>
+      <c r="B538" t="s">
+        <v>0</v>
+      </c>
+      <c r="C538" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D538" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E538" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F538" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G538" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H538" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="s">
+        <v>198</v>
+      </c>
+      <c r="B539" t="s">
+        <v>0</v>
+      </c>
+      <c r="C539" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D539" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E539" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F539" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G539" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H539" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="s">
+        <v>198</v>
+      </c>
+      <c r="B540" t="s">
+        <v>0</v>
+      </c>
+      <c r="C540" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D540" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E540" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F540" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G540" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H540" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="s">
+        <v>198</v>
+      </c>
+      <c r="B541" t="s">
+        <v>0</v>
+      </c>
+      <c r="C541" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D541" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E541" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F541" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G541" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H541" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="s">
+        <v>199</v>
+      </c>
+      <c r="B542" t="s">
+        <v>0</v>
+      </c>
+      <c r="C542" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D542" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E542" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F542" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G542" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H542" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="s">
+        <v>199</v>
+      </c>
+      <c r="B543" t="s">
+        <v>0</v>
+      </c>
+      <c r="C543" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D543" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E543" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F543" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G543" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H543" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="s">
+        <v>199</v>
+      </c>
+      <c r="B544" t="s">
+        <v>0</v>
+      </c>
+      <c r="C544" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D544" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E544" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F544" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G544" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H544" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="s">
+        <v>200</v>
+      </c>
+      <c r="B545" t="s">
+        <v>0</v>
+      </c>
+      <c r="C545" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D545" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E545" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F545" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G545" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H545" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="s">
+        <v>200</v>
+      </c>
+      <c r="B546" t="s">
+        <v>0</v>
+      </c>
+      <c r="C546" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D546" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E546" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F546" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G546" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H546" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="s">
+        <v>200</v>
+      </c>
+      <c r="B547" t="s">
+        <v>0</v>
+      </c>
+      <c r="C547" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D547" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E547" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F547" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G547" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H547" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="s">
+        <v>201</v>
+      </c>
+      <c r="B548" t="s">
+        <v>0</v>
+      </c>
+      <c r="C548" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D548" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E548" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F548" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G548" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H548" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="s">
+        <v>201</v>
+      </c>
+      <c r="B549" t="s">
+        <v>0</v>
+      </c>
+      <c r="C549" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D549" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E549" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F549" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G549" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H549" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="s">
+        <v>201</v>
+      </c>
+      <c r="B550" t="s">
+        <v>0</v>
+      </c>
+      <c r="C550" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D550" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E550" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F550" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G550" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H550" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="s">
+        <v>202</v>
+      </c>
+      <c r="B551" t="s">
+        <v>0</v>
+      </c>
+      <c r="C551" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D551" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E551" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F551" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G551" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H551" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="s">
+        <v>202</v>
+      </c>
+      <c r="B552" t="s">
+        <v>0</v>
+      </c>
+      <c r="C552" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D552" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E552" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F552" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G552" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H552" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="s">
+        <v>202</v>
+      </c>
+      <c r="B553" t="s">
+        <v>0</v>
+      </c>
+      <c r="C553" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D553" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E553" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F553" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G553" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H553" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="s">
+        <v>203</v>
+      </c>
+      <c r="B554" t="s">
+        <v>0</v>
+      </c>
+      <c r="C554" t="n">
+        <v>1.914729089E9</v>
+      </c>
+      <c r="D554" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E554" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F554" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G554" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H554" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="s">
+        <v>203</v>
+      </c>
+      <c r="B555" t="s">
+        <v>0</v>
+      </c>
+      <c r="C555" t="n">
+        <v>1.914726672E9</v>
+      </c>
+      <c r="D555" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E555" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F555" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G555" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H555" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="s">
+        <v>203</v>
+      </c>
+      <c r="B556" t="s">
+        <v>0</v>
+      </c>
+      <c r="C556" t="n">
+        <v>1.914728742E9</v>
+      </c>
+      <c r="D556" t="n">
+        <v>10012.0</v>
+      </c>
+      <c r="E556" t="n">
+        <v>2.696274E8</v>
+      </c>
+      <c r="F556" t="n">
+        <v>256.0</v>
+      </c>
+      <c r="G556" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="H556" t="n">
+        <v>8193.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>